<commit_message>
Made self-review and corrected some faults, added some info.
</commit_message>
<xml_diff>
--- a/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/Bill of Materials-WSBR_Board(default).xlsx
+++ b/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/Bill of Materials-WSBR_Board(default).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe2074dc24c052ba/Beruflich/TBZ/Projects/Wireless-ScoreBoard/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80E54017-4988-4475-9F3B-8BF2F8024087}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D33300C-B7BD-4242-9A6E-3661368D7D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="16230" xr2:uid="{EA63F4CF-E900-4ADD-AC23-7FB303FA917E}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="12682" xr2:uid="{BB763F71-17A1-44F6-8B5A-BB3C3C670C97}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WSBR_Board(de" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="174">
   <si>
     <t>Fitted</t>
   </si>
@@ -60,6 +71,27 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>BAT1</t>
+  </si>
+  <si>
+    <t>ICP621333PA</t>
+  </si>
+  <si>
+    <t>240mAh</t>
+  </si>
+  <si>
+    <t>EMECH SINGLE BATTERY LIPO</t>
+  </si>
+  <si>
+    <t>Renata</t>
+  </si>
+  <si>
+    <t>Conrad</t>
+  </si>
+  <si>
+    <t>252027 - UP</t>
+  </si>
+  <si>
     <t>C1, C11, C13, C14, C22</t>
   </si>
   <si>
@@ -171,7 +203,7 @@
     <t>BAS16W-FDICT-ND</t>
   </si>
   <si>
-    <t>D4, D5, D6, D7, D8</t>
+    <t>D4, D6, D7, D8, D9</t>
   </si>
   <si>
     <t>APHHS1005LZGCK-V</t>
@@ -192,7 +224,7 @@
     <t>754-2126-1-ND</t>
   </si>
   <si>
-    <t>D9</t>
+    <t>D5</t>
   </si>
   <si>
     <t>APHF1608SEEQBDZGKC</t>
@@ -252,7 +284,127 @@
     <t>952-M20-8890445RCT-ND</t>
   </si>
   <si>
-    <t>MEC1</t>
+    <t>R1, R2, R3, R4</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>5k1</t>
+  </si>
+  <si>
+    <t>RES 5k1 62.5mW 1% 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-075K1L</t>
+  </si>
+  <si>
+    <t>311-5.10KLRCT-ND</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>1k6</t>
+  </si>
+  <si>
+    <t>RES 1k6 62.5mW 1% 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-071K6L</t>
+  </si>
+  <si>
+    <t>YAG3045CT-ND</t>
+  </si>
+  <si>
+    <t>R6, R7, R9, R10, R11</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RES 10k 62.5mW 1% 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>311-10.0KLRCT-ND</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>NCU15XH103F6SRC</t>
+  </si>
+  <si>
+    <t>10k 3380K</t>
+  </si>
+  <si>
+    <t>RES NTC 10k 3380K</t>
+  </si>
+  <si>
+    <t>490-NCU15XH103F6SRCCT-ND</t>
+  </si>
+  <si>
+    <t>R12, R15, R16</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>RES 0R 0603</t>
+  </si>
+  <si>
+    <t>YAEGO</t>
+  </si>
+  <si>
+    <t>RC0603FR-070RL</t>
+  </si>
+  <si>
+    <t>311-0.0HRCT-ND</t>
+  </si>
+  <si>
+    <t>Not Fitted</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>RES 220R 62.5mW 1% 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-07220RL</t>
+  </si>
+  <si>
+    <t>311-220LRCT-ND</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>68R</t>
+  </si>
+  <si>
+    <t>RES 68R 0603</t>
+  </si>
+  <si>
+    <t>RC0603FR-0768RL</t>
+  </si>
+  <si>
+    <t>311-68.0HRCT-ND</t>
+  </si>
+  <si>
+    <t>R17, R18, R19, R20</t>
+  </si>
+  <si>
+    <t>S1</t>
   </si>
   <si>
     <t>MG001V</t>
@@ -270,145 +422,7 @@
     <t>MG001V / 3 Key RYG</t>
   </si>
   <si>
-    <t>MEC2</t>
-  </si>
-  <si>
-    <t>ICP621333PA</t>
-  </si>
-  <si>
-    <t>EMECH SINGLE BATTERY LIPO</t>
-  </si>
-  <si>
-    <t>Renata</t>
-  </si>
-  <si>
-    <t>Conrad</t>
-  </si>
-  <si>
-    <t>252027 - UP</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4</t>
-  </si>
-  <si>
-    <t>R0402</t>
-  </si>
-  <si>
-    <t>5k1</t>
-  </si>
-  <si>
-    <t>RES 5k1 62.5mW 1% 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-075K1L</t>
-  </si>
-  <si>
-    <t>311-5.10KLRCT-ND</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>1k6</t>
-  </si>
-  <si>
-    <t>RES 1k6 62.5mW 1% 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-071K6L</t>
-  </si>
-  <si>
-    <t>YAG3045CT-ND</t>
-  </si>
-  <si>
-    <t>R6, R7, R9, R10, R11</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RES 10k 62.5mW 1% 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t>311-10.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>NCU15XH103F6SRC</t>
-  </si>
-  <si>
-    <t>10k 3380K</t>
-  </si>
-  <si>
-    <t>RES NTC 10k 3380K</t>
-  </si>
-  <si>
-    <t>490-NCU15XH103F6SRCCT-ND</t>
-  </si>
-  <si>
-    <t>R12, R15, R16</t>
-  </si>
-  <si>
-    <t>R0603</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>RES 0R 0603</t>
-  </si>
-  <si>
-    <t>YAEGO</t>
-  </si>
-  <si>
-    <t>RC0603FR-070RL</t>
-  </si>
-  <si>
-    <t>311-0.0HRCT-ND</t>
-  </si>
-  <si>
-    <t>Not Fitted</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>RES 220R 62.5mW 1% 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-07220RL</t>
-  </si>
-  <si>
-    <t>311-220LRCT-ND</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>68R</t>
-  </si>
-  <si>
-    <t>RES 68R 0603</t>
-  </si>
-  <si>
-    <t>RC0603FR-0768RL</t>
-  </si>
-  <si>
-    <t>311-68.0HRCT-ND</t>
-  </si>
-  <si>
-    <t>R17, R18, R19, R20</t>
-  </si>
-  <si>
-    <t>S1, S2, S4</t>
+    <t>S2, S3, S5</t>
   </si>
   <si>
     <t>PTS636</t>
@@ -426,7 +440,7 @@
     <t>CKN12311-1-ND</t>
   </si>
   <si>
-    <t>S3</t>
+    <t>S4</t>
   </si>
   <si>
     <t>OS102011MS2QN1</t>
@@ -438,7 +452,7 @@
     <t>CKN9565-ND</t>
   </si>
   <si>
-    <t>TP15</t>
+    <t>TP3, TP4</t>
   </si>
   <si>
     <t>5019</t>
@@ -557,7 +571,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -611,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,7 +641,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -637,39 +651,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -721,7 +735,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -832,13 +846,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -847,6 +854,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -911,29 +925,48 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497E8688-A070-484F-B131-9F9C418738F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9006578-4334-494B-A0D5-F649EA93BD1B}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="1" max="10" width="18.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -965,7 +998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -985,83 +1018,83 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="J4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1069,127 +1102,127 @@
         <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>53</v>
       </c>
       <c r="J8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1199,187 +1232,191 @@
       <c r="C9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" s="1">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="E14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>88</v>
@@ -1388,22 +1425,22 @@
         <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>91</v>
       </c>
       <c r="J15" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1448,7 @@
         <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>93</v>
@@ -1420,22 +1457,22 @@
         <v>94</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>95</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>96</v>
       </c>
       <c r="J16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -1443,31 +1480,31 @@
         <v>97</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>101</v>
       </c>
       <c r="J17" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1484,62 +1521,62 @@
         <v>105</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J19" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>115</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>116</v>
@@ -1548,22 +1585,22 @@
         <v>117</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>118</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>119</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -1571,370 +1608,370 @@
         <v>120</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J21" s="1">
+      <c r="G22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J22" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J23" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J24" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="H25" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="H26" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J26" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="H27" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="H28" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="H29" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="H30" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J30" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="H31" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J31" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="H32" s="2" t="s">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J32" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added debounce C's for S1 and S3.
</commit_message>
<xml_diff>
--- a/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/Bill of Materials-WSBR_Board(default).xlsx
+++ b/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/Bill of Materials-WSBR_Board(default).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe2074dc24c052ba/Beruflich/TBZ/Projects/Wireless-ScoreBoard/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D33300C-B7BD-4242-9A6E-3661368D7D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB585447-CC2E-4385-96AC-DFBAEEC3D210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="12682" xr2:uid="{BB763F71-17A1-44F6-8B5A-BB3C3C670C97}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="12682" xr2:uid="{0173CD5D-68DF-44F0-AC15-6AC1DF1F6F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WSBR_Board(de" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <t>311-1885-1-ND</t>
   </si>
   <si>
-    <t>C2, C3, C6, C9, C12, C15, C16, C17, C19, C20, C21</t>
+    <t>C2, C3, C6, C9, C12, C15, C16, C17, C19, C20, C21, C23, C24, C25, C26</t>
   </si>
   <si>
     <t>C0402</t>
@@ -956,7 +956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9006578-4334-494B-A0D5-F649EA93BD1B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE9B1D1-C3E7-4101-871E-864583D4DD04}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1091,7 +1091,7 @@
         <v>30</v>
       </c>
       <c r="J4" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Schematic changes according to review.
</commit_message>
<xml_diff>
--- a/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/Bill of Materials-WSBR_Board(default).xlsx
+++ b/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/Bill of Materials-WSBR_Board(default).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27504"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe2074dc24c052ba/Beruflich/TBZ/Projects/Wireless-ScoreBoard/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe2074dc24c052ba/Beruflich/TBZ/Projects/Wireless-ScoreBoard-Remote/5_Hardware/WSBR_Board/Project Outputs for WSBR_Board/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB585447-CC2E-4385-96AC-DFBAEEC3D210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AABBCAA2-F1DA-4138-B6B6-EE4F688FC253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="12682" xr2:uid="{0173CD5D-68DF-44F0-AC15-6AC1DF1F6F0A}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="21600" windowHeight="12682" xr2:uid="{77084BB7-CFE8-4C88-893F-6F305E2DAE0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WSBR_Board(de" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-WSBR_Board(de'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="185">
   <si>
     <t>Fitted</t>
   </si>
@@ -134,7 +134,7 @@
     <t>311-3566-1-ND</t>
   </si>
   <si>
-    <t>C4</t>
+    <t>C4, C27</t>
   </si>
   <si>
     <t>C1206</t>
@@ -185,7 +185,7 @@
     <t>311-1884-1-ND</t>
   </si>
   <si>
-    <t>D1, D2, D3</t>
+    <t>D1, D2, D3, D10</t>
   </si>
   <si>
     <t>BAS16W-7-F</t>
@@ -284,6 +284,39 @@
     <t>952-M20-8890445RCT-ND</t>
   </si>
   <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>VZ43FC</t>
+  </si>
+  <si>
+    <t>EMECH VIBRATION MOTOR 3V</t>
+  </si>
+  <si>
+    <t>Vybronics Inc</t>
+  </si>
+  <si>
+    <t>VZ43FC1B5640007L</t>
+  </si>
+  <si>
+    <t>1670-VZ43FC1B5640007LCT-ND</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>BSS138</t>
+  </si>
+  <si>
+    <t>MOSFET N 0.2A 50V SOT323</t>
+  </si>
+  <si>
+    <t>BSS138W-7-F</t>
+  </si>
+  <si>
+    <t>BSS138W-FDICT-ND</t>
+  </si>
+  <si>
     <t>R1, R2, R3, R4</t>
   </si>
   <si>
@@ -302,7 +335,7 @@
     <t>311-5.10KLRCT-ND</t>
   </si>
   <si>
-    <t>R5</t>
+    <t>R5, R21</t>
   </si>
   <si>
     <t>1k6</t>
@@ -317,7 +350,7 @@
     <t>YAG3045CT-ND</t>
   </si>
   <si>
-    <t>R6, R7, R9, R10, R11</t>
+    <t>R6, R7, R9, R10, R11, R22</t>
   </si>
   <si>
     <t>10k</t>
@@ -554,20 +587,20 @@
     <t>U8</t>
   </si>
   <si>
-    <t>nRF24L01 SMD</t>
-  </si>
-  <si>
-    <t>RF Module SPI</t>
-  </si>
-  <si>
-    <t>Nordic Semiconductor ASA</t>
+    <t>HC-12</t>
+  </si>
+  <si>
+    <t>RF Module UART</t>
+  </si>
+  <si>
+    <t>HC Tech</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -956,17 +989,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE9B1D1-C3E7-4101-871E-864583D4DD04}">
-  <dimension ref="A1:J32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4530E1E4-F58E-4250-AE78-71B44E13D641}">
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="10" width="18.53125" customWidth="1"/>
+    <col min="1" max="10" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -998,7 +1031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1094,7 +1127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1123,10 +1156,10 @@
         <v>37</v>
       </c>
       <c r="J5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1219,10 +1252,10 @@
         <v>53</v>
       </c>
       <c r="J8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1346,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1386,14 +1419,12 @@
       <c r="C14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>85</v>
@@ -1405,10 +1436,10 @@
         <v>86</v>
       </c>
       <c r="J14" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1416,16 +1447,14 @@
         <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>90</v>
@@ -1440,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -1448,39 +1477,39 @@
         <v>92</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J16" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>99</v>
@@ -1489,30 +1518,30 @@
         <v>100</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>104</v>
@@ -1521,71 +1550,71 @@
         <v>105</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J18" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>118</v>
@@ -1597,376 +1626,440 @@
         <v>119</v>
       </c>
       <c r="J20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J21" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="E22" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="J22" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>130</v>
+        <v>21</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="J23" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>23</v>
+        <v>136</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J25" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="H26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="H27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>153</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="H28" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="H29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="H30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="J30" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="J31" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E32" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="H32" s="2" t="s">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="J32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J34" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>